<commit_message>
Bugfix for detectSign, it now handles the case in which an homography can't be computed
Refers to #12
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\doc\AESD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{93E4632E-76D3-4F7E-BE9F-01313A42DFFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE7D502-9984-4BB3-BD34-6A211FE5203B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="2265" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3855" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -37,19 +37,13 @@
     <t>LED?</t>
   </si>
   <si>
-    <t>breaks</t>
-  </si>
-  <si>
-    <t>LED? Breaks</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,11 +877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,8 +965,8 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,9 +1001,6 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1029,8 +1020,8 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
+      <c r="C12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,8 +1042,8 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,8 +1053,8 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
+      <c r="C15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,8 +1064,8 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
+      <c r="C16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,8 +1097,11 @@
       <c r="B19">
         <v>2</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1117,8 +1111,8 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
+      <c r="C20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,8 +1133,8 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>5</v>
+      <c r="C22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>